<commit_message>
feat: Add test results of iAsk and you.com
</commit_message>
<xml_diff>
--- a/evaluations/promptfoo/ambiguity_search/20240925-felo.xlsx
+++ b/evaluations/promptfoo/ambiguity_search/20240925-felo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\code\github\ASEED\evaluations\promptfoo\ambiguity_search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2E5172-9635-40B2-A031-0CE6FDBC19D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF1C555-EDB3-4834-99D1-0C5D81BB78F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Google Ranking API 1美元1000次</t>
-  </si>
-  <si>
-    <t>Knowledge Bases for Amazon Bedrock的自動數據同步功能是Amazon Bedrock的一項功能，它用於自動保持用戶在查詢時使用的知識庫處於最新狀態。當用戶上傳數據源以建立知識庫時，該數據源將定期自動同步，使知識庫反映最新信息。這樣一來，用戶就可以始終使用最新信息來增強根據模型的響應生成。</t>
   </si>
   <si>
     <t>融资120万美元</t>
@@ -592,6 +589,16 @@
   </si>
   <si>
     <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Felo.ai 的用户满意度总体上是非常高的。以下是一些关键点：
+高准确度和实用性：用户对 Felo.ai 的搜索结果准确性和实用性表示满意，认为其在深度研究和数据查找方面表现出色。
+多语言支持：Felo.ai 支持多种语言，包括英语、简体中文、繁体中文、日语、韩语、法语、西班牙语、德语、俄语、意大利语、印尼语、泰语和捷克语等，这有助于用户突破语言障碍，更便捷地获取全球信息。
+实时新闻搜索功能：用户对 Felo.ai 的实时新闻搜索功能表示认可，认为其能够快速回答迫切需要了解的问题。
+用户界面和操作简便：Felo.ai 的用户界面简洁，操作步骤简单，适合各种场景下的跨语言交流。
+免费使用：用户对 Felo.ai 的免费使用政策表示赞赏，认为这使得其服务更加亲民。
+此外，Felo.ai 的 AI 驱动搜索技术在搜索准确性、用户体验、转化率和客户满意度方面都有显著改善。这些因素共同提升了用户对 Felo.ai 的满意度。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -678,11 +685,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -702,6 +706,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1043,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1072,292 +1082,292 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="D15" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="D16" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="D18" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>68</v>
+      <c r="D21" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="8">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7">
         <v>0.8</v>
       </c>
       <c r="E23" t="s">

</xml_diff>